<commit_message>
Including notification data from 2014
</commit_message>
<xml_diff>
--- a/data/excelsheets/agesexnotifications.xlsx
+++ b/data/excelsheets/agesexnotifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="30">
   <si>
     <t>00-04</t>
   </si>
@@ -106,6 +106,9 @@
   <si>
     <t>Recent and unspecified infections have also been combied</t>
   </si>
+  <si>
+    <t>Last updated 8/4/2015</t>
+  </si>
 </sst>
 </file>
 
@@ -149,10 +152,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B7"/>
+  <dimension ref="B2:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,6 +494,11 @@
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -498,15 +511,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T41"/>
+  <dimension ref="A2:U42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -567,8 +578,11 @@
       <c r="T2">
         <v>2013</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -648,8 +662,12 @@
         <f>ROUND(TotalCalcSheet!T3*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T48*(1+TotalCalcSheet!T$67), 0)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3" s="7">
+        <f>ROUND(TotalCalcSheet!U3*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U48*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -729,8 +747,12 @@
         <f>ROUND(TotalCalcSheet!T4*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T49*(1+TotalCalcSheet!T$67), 0)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="7">
+        <f>ROUND(TotalCalcSheet!U4*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U49*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -810,8 +832,12 @@
         <f>ROUND(TotalCalcSheet!T5*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T50*(1+TotalCalcSheet!T$67), 0)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="7">
+        <f>ROUND(TotalCalcSheet!U5*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U50*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -891,8 +917,12 @@
         <f>ROUND(TotalCalcSheet!T6*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T51*(1+TotalCalcSheet!T$67), 0)</f>
         <v>186</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="7">
+        <f>ROUND(TotalCalcSheet!U6*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U51*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -972,8 +1002,12 @@
         <f>ROUND(TotalCalcSheet!T7*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T52*(1+TotalCalcSheet!T$67), 0)</f>
         <v>678</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="7">
+        <f>ROUND(TotalCalcSheet!U7*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U52*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1053,8 +1087,12 @@
         <f>ROUND(TotalCalcSheet!T8*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T53*(1+TotalCalcSheet!T$67), 0)</f>
         <v>842</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="7">
+        <f>ROUND(TotalCalcSheet!U8*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U53*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1134,8 +1172,12 @@
         <f>ROUND(TotalCalcSheet!T9*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T54*(1+TotalCalcSheet!T$67), 0)</f>
         <v>985</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="7">
+        <f>ROUND(TotalCalcSheet!U9*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U54*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1215,8 +1257,12 @@
         <f>ROUND(TotalCalcSheet!T10*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T55*(1+TotalCalcSheet!T$67), 0)</f>
         <v>895</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="7">
+        <f>ROUND(TotalCalcSheet!U10*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U55*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>923</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1296,8 +1342,12 @@
         <f>ROUND(TotalCalcSheet!T11*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T56*(1+TotalCalcSheet!T$67), 0)</f>
         <v>880</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="7">
+        <f>ROUND(TotalCalcSheet!U11*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U56*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>906</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1377,8 +1427,12 @@
         <f>ROUND(TotalCalcSheet!T12*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T57*(1+TotalCalcSheet!T$67), 0)</f>
         <v>829</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="7">
+        <f>ROUND(TotalCalcSheet!U12*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U57*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>811</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1458,8 +1512,12 @@
         <f>ROUND(TotalCalcSheet!T13*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T58*(1+TotalCalcSheet!T$67), 0)</f>
         <v>716</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="7">
+        <f>ROUND(TotalCalcSheet!U13*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U58*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1539,8 +1597,12 @@
         <f>ROUND(TotalCalcSheet!T14*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T59*(1+TotalCalcSheet!T$67), 0)</f>
         <v>580</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="7">
+        <f>ROUND(TotalCalcSheet!U14*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U59*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>654</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1620,8 +1682,12 @@
         <f>ROUND(TotalCalcSheet!T15*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T60*(1+TotalCalcSheet!T$67), 0)</f>
         <v>265</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" s="7">
+        <f>ROUND(TotalCalcSheet!U15*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U60*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1701,8 +1767,12 @@
         <f>ROUND(TotalCalcSheet!T16*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T61*(1+TotalCalcSheet!T$67), 0)</f>
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16" s="7">
+        <f>ROUND(TotalCalcSheet!U16*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U61*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1782,8 +1852,12 @@
         <f>ROUND(TotalCalcSheet!T17*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T62*(1+TotalCalcSheet!T$67), 0)</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="7">
+        <f>ROUND(TotalCalcSheet!U17*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U62*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1863,8 +1937,12 @@
         <f>ROUND(TotalCalcSheet!T18*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T63*(1+TotalCalcSheet!T$67), 0)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="7">
+        <f>ROUND(TotalCalcSheet!U18*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U63*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1944,8 +2022,12 @@
         <f>ROUND(TotalCalcSheet!T19*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T64*(1+TotalCalcSheet!T$67), 0)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="7">
+        <f>ROUND(TotalCalcSheet!U19*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U64*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2025,8 +2107,15 @@
         <f>ROUND(TotalCalcSheet!T20*(1+TotalCalcSheet!T$22)+TotalCalcSheet!T65*(1+TotalCalcSheet!T$67), 0)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20" s="7">
+        <f>ROUND(TotalCalcSheet!U20*(1+TotalCalcSheet!U$22)+TotalCalcSheet!U65*(1+TotalCalcSheet!U$67), 0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U21" s="7"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2106,8 +2195,12 @@
         <f t="shared" si="0"/>
         <v>2013</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U23" s="7">
+        <f t="shared" ref="U23" si="1">U2</f>
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>A3</f>
         <v>00-04</v>
@@ -2188,10 +2281,14 @@
         <f>ROUND(TotalCalcSheet!T25*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T70*(1+TotalCalcSheet!T$89), 0)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24" s="7">
+        <f>ROUND(TotalCalcSheet!U25*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U70*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="shared" ref="A25:A42" si="1">A4</f>
+        <f t="shared" ref="A25:A41" si="2">A4</f>
         <v>05-09</v>
       </c>
       <c r="B25">
@@ -2270,10 +2367,14 @@
         <f>ROUND(TotalCalcSheet!T26*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T71*(1+TotalCalcSheet!T$89), 0)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U25" s="7">
+        <f>ROUND(TotalCalcSheet!U26*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U71*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10-14</v>
       </c>
       <c r="B26">
@@ -2352,10 +2453,14 @@
         <f>ROUND(TotalCalcSheet!T27*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T72*(1+TotalCalcSheet!T$89), 0)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U26" s="7">
+        <f>ROUND(TotalCalcSheet!U27*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U72*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15-19</v>
       </c>
       <c r="B27">
@@ -2434,10 +2539,14 @@
         <f>ROUND(TotalCalcSheet!T28*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T73*(1+TotalCalcSheet!T$89), 0)</f>
         <v>135</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U27" s="7">
+        <f>ROUND(TotalCalcSheet!U28*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U73*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20-24</v>
       </c>
       <c r="B28">
@@ -2516,10 +2625,14 @@
         <f>ROUND(TotalCalcSheet!T29*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T74*(1+TotalCalcSheet!T$89), 0)</f>
         <v>362</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U28" s="7">
+        <f>ROUND(TotalCalcSheet!U29*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U74*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25-29</v>
       </c>
       <c r="B29">
@@ -2598,10 +2711,14 @@
         <f>ROUND(TotalCalcSheet!T30*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T75*(1+TotalCalcSheet!T$89), 0)</f>
         <v>413</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U29" s="7">
+        <f>ROUND(TotalCalcSheet!U30*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U75*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30-34</v>
       </c>
       <c r="B30">
@@ -2680,10 +2797,14 @@
         <f>ROUND(TotalCalcSheet!T31*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T76*(1+TotalCalcSheet!T$89), 0)</f>
         <v>610</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U30" s="7">
+        <f>ROUND(TotalCalcSheet!U31*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U76*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>537</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35-39</v>
       </c>
       <c r="B31">
@@ -2762,10 +2883,14 @@
         <f>ROUND(TotalCalcSheet!T32*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T77*(1+TotalCalcSheet!T$89), 0)</f>
         <v>458</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U31" s="7">
+        <f>ROUND(TotalCalcSheet!U32*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U77*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>465</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40-44</v>
       </c>
       <c r="B32">
@@ -2844,10 +2969,14 @@
         <f>ROUND(TotalCalcSheet!T33*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T78*(1+TotalCalcSheet!T$89), 0)</f>
         <v>389</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U32" s="7">
+        <f>ROUND(TotalCalcSheet!U33*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U78*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>423</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45-49</v>
       </c>
       <c r="B33">
@@ -2926,10 +3055,14 @@
         <f>ROUND(TotalCalcSheet!T34*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T79*(1+TotalCalcSheet!T$89), 0)</f>
         <v>362</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U33" s="7">
+        <f>ROUND(TotalCalcSheet!U34*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U79*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50-54</v>
       </c>
       <c r="B34">
@@ -3008,10 +3141,14 @@
         <f>ROUND(TotalCalcSheet!T35*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T80*(1+TotalCalcSheet!T$89), 0)</f>
         <v>368</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U34" s="7">
+        <f>ROUND(TotalCalcSheet!U35*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U80*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55-59</v>
       </c>
       <c r="B35">
@@ -3090,10 +3227,14 @@
         <f>ROUND(TotalCalcSheet!T36*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T81*(1+TotalCalcSheet!T$89), 0)</f>
         <v>286</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U35" s="7">
+        <f>ROUND(TotalCalcSheet!U36*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U81*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60-64</v>
       </c>
       <c r="B36">
@@ -3172,10 +3313,14 @@
         <f>ROUND(TotalCalcSheet!T37*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T82*(1+TotalCalcSheet!T$89), 0)</f>
         <v>117</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U36" s="7">
+        <f>ROUND(TotalCalcSheet!U37*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U82*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65-69</v>
       </c>
       <c r="B37">
@@ -3254,10 +3399,14 @@
         <f>ROUND(TotalCalcSheet!T38*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T83*(1+TotalCalcSheet!T$89), 0)</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U37" s="7">
+        <f>ROUND(TotalCalcSheet!U38*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U83*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70-74</v>
       </c>
       <c r="B38">
@@ -3336,10 +3485,14 @@
         <f>ROUND(TotalCalcSheet!T39*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T84*(1+TotalCalcSheet!T$89), 0)</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U38" s="7">
+        <f>ROUND(TotalCalcSheet!U39*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U84*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75-79</v>
       </c>
       <c r="B39">
@@ -3418,10 +3571,14 @@
         <f>ROUND(TotalCalcSheet!T40*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T85*(1+TotalCalcSheet!T$89), 0)</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U39" s="7">
+        <f>ROUND(TotalCalcSheet!U40*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U85*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80-84</v>
       </c>
       <c r="B40">
@@ -3500,10 +3657,14 @@
         <f>ROUND(TotalCalcSheet!T41*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T86*(1+TotalCalcSheet!T$89), 0)</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U40" s="7">
+        <f>ROUND(TotalCalcSheet!U41*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U86*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>85+</v>
       </c>
       <c r="B41">
@@ -3582,6 +3743,14 @@
         <f>ROUND(TotalCalcSheet!T42*(1+TotalCalcSheet!T$44)+TotalCalcSheet!T87*(1+TotalCalcSheet!T$89), 0)</f>
         <v>22</v>
       </c>
+      <c r="U41" s="7">
+        <f>ROUND(TotalCalcSheet!U42*(1+TotalCalcSheet!U$44)+TotalCalcSheet!U87*(1+TotalCalcSheet!U$89), 0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T42" s="7"/>
+      <c r="U42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3590,10 +3759,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T89"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3601,12 +3770,12 @@
     <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3667,8 +3836,11 @@
       <c r="T2">
         <v>2013</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" s="7">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3748,8 +3920,12 @@
         <f>'unspecified-originaldata'!T2+'unspecified-originaldata'!T44*0.66</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3" s="7">
+        <f>'unspecified-originaldata'!U2+'unspecified-originaldata'!U44*0.66</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -3829,8 +4005,12 @@
         <f>'unspecified-originaldata'!T3+'unspecified-originaldata'!T45*0.66</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="7">
+        <f>'unspecified-originaldata'!U3+'unspecified-originaldata'!U45*0.66</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -3910,8 +4090,12 @@
         <f>'unspecified-originaldata'!T4+'unspecified-originaldata'!T46*0.66</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="7">
+        <f>'unspecified-originaldata'!U4+'unspecified-originaldata'!U46*0.66</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3991,8 +4175,12 @@
         <f>'unspecified-originaldata'!T5+'unspecified-originaldata'!T47*0.66</f>
         <v>158.66</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="7">
+        <f>'unspecified-originaldata'!U5+'unspecified-originaldata'!U47*0.66</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -4072,8 +4260,12 @@
         <f>'unspecified-originaldata'!T6+'unspecified-originaldata'!T48*0.66</f>
         <v>613.64</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7" s="7">
+        <f>'unspecified-originaldata'!U6+'unspecified-originaldata'!U48*0.66</f>
+        <v>541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -4153,8 +4345,12 @@
         <f>'unspecified-originaldata'!T7+'unspecified-originaldata'!T49*0.66</f>
         <v>777.66</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8" s="7">
+        <f>'unspecified-originaldata'!U7+'unspecified-originaldata'!U49*0.66</f>
+        <v>778.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -4234,8 +4430,12 @@
         <f>'unspecified-originaldata'!T8+'unspecified-originaldata'!T50*0.66</f>
         <v>938.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="7">
+        <f>'unspecified-originaldata'!U8+'unspecified-originaldata'!U50*0.66</f>
+        <v>963.96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4315,8 +4515,12 @@
         <f>'unspecified-originaldata'!T9+'unspecified-originaldata'!T51*0.66</f>
         <v>871.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="7">
+        <f>'unspecified-originaldata'!U9+'unspecified-originaldata'!U51*0.66</f>
+        <v>898.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -4396,8 +4600,12 @@
         <f>'unspecified-originaldata'!T10+'unspecified-originaldata'!T52*0.66</f>
         <v>852.98</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="7">
+        <f>'unspecified-originaldata'!U10+'unspecified-originaldata'!U52*0.66</f>
+        <v>884.32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -4477,8 +4685,12 @@
         <f>'unspecified-originaldata'!T11+'unspecified-originaldata'!T53*0.66</f>
         <v>811.66</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12" s="7">
+        <f>'unspecified-originaldata'!U11+'unspecified-originaldata'!U53*0.66</f>
+        <v>792.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -4558,8 +4770,12 @@
         <f>'unspecified-originaldata'!T12+'unspecified-originaldata'!T54*0.66</f>
         <v>711</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13" s="7">
+        <f>'unspecified-originaldata'!U12+'unspecified-originaldata'!U54*0.66</f>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -4639,8 +4855,12 @@
         <f>'unspecified-originaldata'!T13+'unspecified-originaldata'!T55*0.66</f>
         <v>571.66</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14" s="7">
+        <f>'unspecified-originaldata'!U13+'unspecified-originaldata'!U55*0.66</f>
+        <v>645.98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -4720,8 +4940,12 @@
         <f>'unspecified-originaldata'!T14+'unspecified-originaldata'!T56*0.66</f>
         <v>263</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15" s="7">
+        <f>'unspecified-originaldata'!U14+'unspecified-originaldata'!U56*0.66</f>
+        <v>298.66000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -4801,8 +5025,12 @@
         <f>'unspecified-originaldata'!T15+'unspecified-originaldata'!T57*0.66</f>
         <v>85.66</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16" s="7">
+        <f>'unspecified-originaldata'!U15+'unspecified-originaldata'!U57*0.66</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -4882,8 +5110,12 @@
         <f>'unspecified-originaldata'!T16+'unspecified-originaldata'!T58*0.66</f>
         <v>28.66</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17" s="7">
+        <f>'unspecified-originaldata'!U16+'unspecified-originaldata'!U58*0.66</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -4963,8 +5195,12 @@
         <f>'unspecified-originaldata'!T17+'unspecified-originaldata'!T59*0.66</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18" s="7">
+        <f>'unspecified-originaldata'!U17+'unspecified-originaldata'!U59*0.66</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -5044,8 +5280,12 @@
         <f>'unspecified-originaldata'!T18+'unspecified-originaldata'!T60*0.66</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19" s="7">
+        <f>'unspecified-originaldata'!U18+'unspecified-originaldata'!U60*0.66</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -5125,8 +5365,12 @@
         <f>'unspecified-originaldata'!T19+'unspecified-originaldata'!T61*0.66</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20" s="7">
+        <f>'unspecified-originaldata'!U19+'unspecified-originaldata'!U61*0.66</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -5206,8 +5450,12 @@
         <f>'unspecified-originaldata'!T20+'unspecified-originaldata'!T62*0.66</f>
         <v>11.32</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U21" s="7">
+        <f>'unspecified-originaldata'!U20+'unspecified-originaldata'!U62*0.66</f>
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -5287,8 +5535,12 @@
         <f t="shared" si="0"/>
         <v>1.6767439173596319E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U22" s="7">
+        <f t="shared" ref="U22" si="1">U21/SUM(U3:U20)</f>
+        <v>9.8619913522478243E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -5297,79 +5549,83 @@
         <v>1995</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:T24" si="1">C2</f>
+        <f t="shared" ref="C24:T24" si="2">C2</f>
         <v>1996</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1997</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1998</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1999</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2001</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2002</v>
       </c>
       <c r="J24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2003</v>
       </c>
       <c r="K24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2004</v>
       </c>
       <c r="L24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2005</v>
       </c>
       <c r="M24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2006</v>
       </c>
       <c r="N24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2007</v>
       </c>
       <c r="O24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2008</v>
       </c>
       <c r="P24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2009</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2010</v>
       </c>
       <c r="R24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2011</v>
       </c>
       <c r="S24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2012</v>
       </c>
       <c r="T24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2013</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24" s="7">
+        <f t="shared" ref="U24" si="3">U2</f>
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>A3</f>
         <v>00-04</v>
@@ -5450,10 +5706,14 @@
         <f>'unspecified-originaldata'!T23+'unspecified-originaldata'!T44*0.33</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U25" s="7">
+        <f>'unspecified-originaldata'!U23+'unspecified-originaldata'!U44*0.33</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="shared" ref="A26:A43" si="2">A4</f>
+        <f t="shared" ref="A26:A43" si="4">A4</f>
         <v>05-09</v>
       </c>
       <c r="B26">
@@ -5532,10 +5792,14 @@
         <f>'unspecified-originaldata'!T24+'unspecified-originaldata'!T45*0.33</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U26" s="7">
+        <f>'unspecified-originaldata'!U24+'unspecified-originaldata'!U45*0.33</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10-14</v>
       </c>
       <c r="B27">
@@ -5614,10 +5878,14 @@
         <f>'unspecified-originaldata'!T25+'unspecified-originaldata'!T46*0.33</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U27" s="7">
+        <f>'unspecified-originaldata'!U25+'unspecified-originaldata'!U46*0.33</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15-19</v>
       </c>
       <c r="B28">
@@ -5696,10 +5964,14 @@
         <f>'unspecified-originaldata'!T26+'unspecified-originaldata'!T47*0.33</f>
         <v>120.33</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U28" s="7">
+        <f>'unspecified-originaldata'!U26+'unspecified-originaldata'!U47*0.33</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20-24</v>
       </c>
       <c r="B29">
@@ -5778,10 +6050,14 @@
         <f>'unspecified-originaldata'!T27+'unspecified-originaldata'!T48*0.33</f>
         <v>330.32</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U29" s="7">
+        <f>'unspecified-originaldata'!U27+'unspecified-originaldata'!U48*0.33</f>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>25-29</v>
       </c>
       <c r="B30">
@@ -5860,10 +6136,14 @@
         <f>'unspecified-originaldata'!T28+'unspecified-originaldata'!T49*0.33</f>
         <v>379.33</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U30" s="7">
+        <f>'unspecified-originaldata'!U28+'unspecified-originaldata'!U49*0.33</f>
+        <v>386.66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>30-34</v>
       </c>
       <c r="B31">
@@ -5942,10 +6222,14 @@
         <f>'unspecified-originaldata'!T29+'unspecified-originaldata'!T50*0.33</f>
         <v>586.65</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U31" s="7">
+        <f>'unspecified-originaldata'!U29+'unspecified-originaldata'!U50*0.33</f>
+        <v>516.98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>35-39</v>
       </c>
       <c r="B32">
@@ -6024,10 +6308,14 @@
         <f>'unspecified-originaldata'!T30+'unspecified-originaldata'!T51*0.33</f>
         <v>450.65</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U32" s="7">
+        <f>'unspecified-originaldata'!U30+'unspecified-originaldata'!U51*0.33</f>
+        <v>451.65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40-44</v>
       </c>
       <c r="B33">
@@ -6106,10 +6394,14 @@
         <f>'unspecified-originaldata'!T31+'unspecified-originaldata'!T52*0.33</f>
         <v>379.99</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U33" s="7">
+        <f>'unspecified-originaldata'!U31+'unspecified-originaldata'!U52*0.33</f>
+        <v>412.66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45-49</v>
       </c>
       <c r="B34">
@@ -6188,10 +6480,14 @@
         <f>'unspecified-originaldata'!T32+'unspecified-originaldata'!T53*0.33</f>
         <v>353.33</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U34" s="7">
+        <f>'unspecified-originaldata'!U32+'unspecified-originaldata'!U53*0.33</f>
+        <v>392.33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>50-54</v>
       </c>
       <c r="B35">
@@ -6270,10 +6566,14 @@
         <f>'unspecified-originaldata'!T33+'unspecified-originaldata'!T54*0.33</f>
         <v>367</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U35" s="7">
+        <f>'unspecified-originaldata'!U33+'unspecified-originaldata'!U54*0.33</f>
+        <v>379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55-59</v>
       </c>
       <c r="B36">
@@ -6352,10 +6652,14 @@
         <f>'unspecified-originaldata'!T34+'unspecified-originaldata'!T55*0.33</f>
         <v>283.33</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U36" s="7">
+        <f>'unspecified-originaldata'!U34+'unspecified-originaldata'!U55*0.33</f>
+        <v>311.99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>60-64</v>
       </c>
       <c r="B37">
@@ -6434,10 +6738,14 @@
         <f>'unspecified-originaldata'!T35+'unspecified-originaldata'!T56*0.33</f>
         <v>117</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U37" s="7">
+        <f>'unspecified-originaldata'!U35+'unspecified-originaldata'!U56*0.33</f>
+        <v>146.33000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>65-69</v>
       </c>
       <c r="B38">
@@ -6516,10 +6824,14 @@
         <f>'unspecified-originaldata'!T36+'unspecified-originaldata'!T57*0.33</f>
         <v>65.33</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U38" s="7">
+        <f>'unspecified-originaldata'!U36+'unspecified-originaldata'!U57*0.33</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>70-74</v>
       </c>
       <c r="B39">
@@ -6598,10 +6910,14 @@
         <f>'unspecified-originaldata'!T37+'unspecified-originaldata'!T58*0.33</f>
         <v>28.33</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U39" s="7">
+        <f>'unspecified-originaldata'!U37+'unspecified-originaldata'!U58*0.33</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>75-79</v>
       </c>
       <c r="B40">
@@ -6680,10 +6996,14 @@
         <f>'unspecified-originaldata'!T38+'unspecified-originaldata'!T59*0.33</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U40" s="7">
+        <f>'unspecified-originaldata'!U38+'unspecified-originaldata'!U59*0.33</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>80-84</v>
       </c>
       <c r="B41">
@@ -6762,10 +7082,14 @@
         <f>'unspecified-originaldata'!T39+'unspecified-originaldata'!T60*0.33</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U41" s="7">
+        <f>'unspecified-originaldata'!U39+'unspecified-originaldata'!U60*0.33</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>85+</v>
       </c>
       <c r="B42">
@@ -6844,10 +7168,14 @@
         <f>'unspecified-originaldata'!T40+'unspecified-originaldata'!T61*0.33</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U42" s="7">
+        <f>'unspecified-originaldata'!U40+'unspecified-originaldata'!U61*0.33</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>Unknown</v>
       </c>
       <c r="B43">
@@ -6926,8 +7254,12 @@
         <f>'unspecified-originaldata'!T41+'unspecified-originaldata'!T62*0.33</f>
         <v>3.66</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U43" s="7">
+        <f>'unspecified-originaldata'!U41+'unspecified-originaldata'!U62*0.33</f>
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -6936,84 +7268,88 @@
         <v>1.0399357311205734E-2</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44" si="3">C43/SUM(C25:C42)</f>
+        <f t="shared" ref="C44" si="5">C43/SUM(C25:C42)</f>
         <v>1.2273847679298379E-2</v>
       </c>
       <c r="D44">
-        <f t="shared" ref="D44" si="4">D43/SUM(D25:D42)</f>
+        <f t="shared" ref="D44" si="6">D43/SUM(D25:D42)</f>
         <v>2.8168079983346014E-3</v>
       </c>
       <c r="E44">
-        <f t="shared" ref="E44" si="5">E43/SUM(E25:E42)</f>
+        <f t="shared" ref="E44" si="7">E43/SUM(E25:E42)</f>
         <v>3.7574623233144807E-3</v>
       </c>
       <c r="F44">
-        <f t="shared" ref="F44" si="6">F43/SUM(F25:F42)</f>
+        <f t="shared" ref="F44" si="8">F43/SUM(F25:F42)</f>
         <v>2.1113862097441385E-3</v>
       </c>
       <c r="G44">
-        <f t="shared" ref="G44" si="7">G43/SUM(G25:G42)</f>
+        <f t="shared" ref="G44" si="9">G43/SUM(G25:G42)</f>
         <v>3.4818598639874449E-3</v>
       </c>
       <c r="H44">
-        <f t="shared" ref="H44" si="8">H43/SUM(H25:H42)</f>
+        <f t="shared" ref="H44" si="10">H43/SUM(H25:H42)</f>
         <v>2.0663464760415505E-3</v>
       </c>
       <c r="I44">
-        <f t="shared" ref="I44" si="9">I43/SUM(I25:I42)</f>
+        <f t="shared" ref="I44" si="11">I43/SUM(I25:I42)</f>
         <v>2.1927087975755419E-3</v>
       </c>
       <c r="J44">
-        <f t="shared" ref="J44" si="10">J43/SUM(J25:J42)</f>
+        <f t="shared" ref="J44" si="12">J43/SUM(J25:J42)</f>
         <v>5.4405962566243359E-4</v>
       </c>
       <c r="K44">
-        <f t="shared" ref="K44" si="11">K43/SUM(K25:K42)</f>
+        <f t="shared" ref="K44" si="13">K43/SUM(K25:K42)</f>
         <v>4.2879532098545744E-4</v>
       </c>
       <c r="L44">
-        <f t="shared" ref="L44" si="12">L43/SUM(L25:L42)</f>
+        <f t="shared" ref="L44" si="14">L43/SUM(L25:L42)</f>
         <v>5.3556446886025919E-4</v>
       </c>
       <c r="M44">
-        <f t="shared" ref="M44" si="13">M43/SUM(M25:M42)</f>
+        <f t="shared" ref="M44" si="15">M43/SUM(M25:M42)</f>
         <v>7.0024415179425884E-4</v>
       </c>
       <c r="N44">
-        <f t="shared" ref="N44" si="14">N43/SUM(N25:N42)</f>
+        <f t="shared" ref="N44" si="16">N43/SUM(N25:N42)</f>
         <v>4.590372673672944E-4</v>
       </c>
       <c r="O44">
-        <f t="shared" ref="O44" si="15">O43/SUM(O25:O42)</f>
+        <f t="shared" ref="O44" si="17">O43/SUM(O25:O42)</f>
         <v>0</v>
       </c>
       <c r="P44">
-        <f t="shared" ref="P44" si="16">P43/SUM(P25:P42)</f>
+        <f t="shared" ref="P44" si="18">P43/SUM(P25:P42)</f>
         <v>8.2305142574953802E-5</v>
       </c>
       <c r="Q44">
-        <f t="shared" ref="Q44" si="17">Q43/SUM(Q25:Q42)</f>
+        <f t="shared" ref="Q44" si="19">Q43/SUM(Q25:Q42)</f>
         <v>8.1989682141807589E-4</v>
       </c>
       <c r="R44">
-        <f t="shared" ref="R44" si="18">R43/SUM(R25:R42)</f>
+        <f t="shared" ref="R44" si="20">R43/SUM(R25:R42)</f>
         <v>1.1434204606351002E-3</v>
       </c>
       <c r="S44">
-        <f t="shared" ref="S44" si="19">S43/SUM(S25:S42)</f>
+        <f t="shared" ref="S44" si="21">S43/SUM(S25:S42)</f>
         <v>9.745379804029272E-5</v>
       </c>
       <c r="T44">
-        <f t="shared" ref="T44" si="20">T43/SUM(T25:T42)</f>
+        <f t="shared" ref="T44:U44" si="22">T43/SUM(T25:T42)</f>
         <v>1.0340180642390785E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U44" s="7">
+        <f t="shared" si="22"/>
+        <v>6.6013145965548511E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -7074,8 +7410,11 @@
       <c r="T47">
         <v>2013</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U47" s="7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -7155,8 +7494,12 @@
         <f>'newlyacquired-originaldata'!T2+'newlyacquired-originaldata'!T44*0.66</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U48" s="7">
+        <f>'newlyacquired-originaldata'!U2+'newlyacquired-originaldata'!U44*0.66</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>19</v>
       </c>
@@ -7236,8 +7579,12 @@
         <f>'newlyacquired-originaldata'!T3+'newlyacquired-originaldata'!T45*0.66</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U49" s="7">
+        <f>'newlyacquired-originaldata'!U3+'newlyacquired-originaldata'!U45*0.66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>20</v>
       </c>
@@ -7317,8 +7664,12 @@
         <f>'newlyacquired-originaldata'!T4+'newlyacquired-originaldata'!T46*0.66</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U50" s="7">
+        <f>'newlyacquired-originaldata'!U4+'newlyacquired-originaldata'!U46*0.66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -7398,8 +7749,12 @@
         <f>'newlyacquired-originaldata'!T5+'newlyacquired-originaldata'!T47*0.66</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U51" s="7">
+        <f>'newlyacquired-originaldata'!U5+'newlyacquired-originaldata'!U47*0.66</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -7479,8 +7834,12 @@
         <f>'newlyacquired-originaldata'!T6+'newlyacquired-originaldata'!T48*0.66</f>
         <v>62.66</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U52" s="7">
+        <f>'newlyacquired-originaldata'!U6+'newlyacquired-originaldata'!U48*0.66</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -7560,8 +7919,12 @@
         <f>'newlyacquired-originaldata'!T7+'newlyacquired-originaldata'!T49*0.66</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U53" s="7">
+        <f>'newlyacquired-originaldata'!U7+'newlyacquired-originaldata'!U49*0.66</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -7641,8 +8004,12 @@
         <f>'newlyacquired-originaldata'!T8+'newlyacquired-originaldata'!T50*0.66</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U54" s="7">
+        <f>'newlyacquired-originaldata'!U8+'newlyacquired-originaldata'!U50*0.66</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -7722,8 +8089,12 @@
         <f>'newlyacquired-originaldata'!T9+'newlyacquired-originaldata'!T51*0.66</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U55" s="7">
+        <f>'newlyacquired-originaldata'!U9+'newlyacquired-originaldata'!U51*0.66</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -7803,8 +8174,12 @@
         <f>'newlyacquired-originaldata'!T10+'newlyacquired-originaldata'!T52*0.66</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U56" s="7">
+        <f>'newlyacquired-originaldata'!U10+'newlyacquired-originaldata'!U52*0.66</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -7884,8 +8259,12 @@
         <f>'newlyacquired-originaldata'!T11+'newlyacquired-originaldata'!T53*0.66</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U57" s="7">
+        <f>'newlyacquired-originaldata'!U11+'newlyacquired-originaldata'!U53*0.66</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -7965,8 +8344,12 @@
         <f>'newlyacquired-originaldata'!T12+'newlyacquired-originaldata'!T54*0.66</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U58" s="7">
+        <f>'newlyacquired-originaldata'!U12+'newlyacquired-originaldata'!U54*0.66</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -8046,8 +8429,12 @@
         <f>'newlyacquired-originaldata'!T13+'newlyacquired-originaldata'!T55*0.66</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U59" s="7">
+        <f>'newlyacquired-originaldata'!U13+'newlyacquired-originaldata'!U55*0.66</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -8127,8 +8514,12 @@
         <f>'newlyacquired-originaldata'!T14+'newlyacquired-originaldata'!T56*0.66</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U60" s="7">
+        <f>'newlyacquired-originaldata'!U14+'newlyacquired-originaldata'!U56*0.66</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -8208,8 +8599,12 @@
         <f>'newlyacquired-originaldata'!T15+'newlyacquired-originaldata'!T57*0.66</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U61" s="7">
+        <f>'newlyacquired-originaldata'!U15+'newlyacquired-originaldata'!U57*0.66</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -8289,8 +8684,12 @@
         <f>'newlyacquired-originaldata'!T16+'newlyacquired-originaldata'!T58*0.66</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U62" s="7">
+        <f>'newlyacquired-originaldata'!U16+'newlyacquired-originaldata'!U58*0.66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -8370,8 +8769,12 @@
         <f>'newlyacquired-originaldata'!T17+'newlyacquired-originaldata'!T59*0.66</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U63" s="7">
+        <f>'newlyacquired-originaldata'!U17+'newlyacquired-originaldata'!U59*0.66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -8451,8 +8854,12 @@
         <f>'newlyacquired-originaldata'!T18+'newlyacquired-originaldata'!T60*0.66</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U64" s="7">
+        <f>'newlyacquired-originaldata'!U18+'newlyacquired-originaldata'!U60*0.66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -8532,8 +8939,12 @@
         <f>'newlyacquired-originaldata'!T19+'newlyacquired-originaldata'!T61*0.66</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U65" s="7">
+        <f>'newlyacquired-originaldata'!U19+'newlyacquired-originaldata'!U61*0.66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -8613,8 +9024,12 @@
         <f>'unspecified-originaldata'!T62+'unspecified-originaldata'!T104*0.66</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U66" s="7">
+        <f>'unspecified-originaldata'!U62+'unspecified-originaldata'!U104*0.66</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -8623,79 +9038,83 @@
         <v>0.10126582278481013</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67" si="21">C66/SUM(C48:C65)</f>
+        <f t="shared" ref="C67" si="23">C66/SUM(C48:C65)</f>
         <v>0.10825858335910919</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67" si="22">D66/SUM(D48:D65)</f>
+        <f t="shared" ref="D67" si="24">D66/SUM(D48:D65)</f>
         <v>0.13044350792695164</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67" si="23">E66/SUM(E48:E65)</f>
+        <f t="shared" ref="E67" si="25">E66/SUM(E48:E65)</f>
         <v>0.1044776119402985</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67" si="24">F66/SUM(F48:F65)</f>
+        <f t="shared" ref="F67" si="26">F66/SUM(F48:F65)</f>
         <v>5.5902357216062612E-2</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67" si="25">G66/SUM(G48:G65)</f>
+        <f t="shared" ref="G67" si="27">G66/SUM(G48:G65)</f>
         <v>4.5081967213114756E-2</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67" si="26">H66/SUM(H48:H65)</f>
+        <f t="shared" ref="H67" si="28">H66/SUM(H48:H65)</f>
         <v>1.4705882352941176E-2</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67" si="27">I66/SUM(I48:I65)</f>
+        <f t="shared" ref="I67" si="29">I66/SUM(I48:I65)</f>
         <v>5.8941412236237181E-2</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67" si="28">J66/SUM(J48:J65)</f>
+        <f t="shared" ref="J67" si="30">J66/SUM(J48:J65)</f>
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67" si="29">K66/SUM(K48:K65)</f>
+        <f t="shared" ref="K67" si="31">K66/SUM(K48:K65)</f>
         <v>0</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67" si="30">L66/SUM(L48:L65)</f>
+        <f t="shared" ref="L67" si="32">L66/SUM(L48:L65)</f>
         <v>4.5248868778280547E-3</v>
       </c>
       <c r="M67">
-        <f t="shared" ref="M67" si="31">M66/SUM(M48:M65)</f>
+        <f t="shared" ref="M67" si="33">M66/SUM(M48:M65)</f>
         <v>0</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67" si="32">N66/SUM(N48:N65)</f>
+        <f t="shared" ref="N67" si="34">N66/SUM(N48:N65)</f>
         <v>1.2875536480686695E-2</v>
       </c>
       <c r="O67">
-        <f t="shared" ref="O67" si="33">O66/SUM(O48:O65)</f>
+        <f t="shared" ref="O67" si="35">O66/SUM(O48:O65)</f>
         <v>0</v>
       </c>
       <c r="P67">
-        <f t="shared" ref="P67" si="34">P66/SUM(P48:P65)</f>
+        <f t="shared" ref="P67" si="36">P66/SUM(P48:P65)</f>
         <v>4.0983606557377051E-3</v>
       </c>
       <c r="Q67">
-        <f t="shared" ref="Q67" si="35">Q66/SUM(Q48:Q65)</f>
+        <f t="shared" ref="Q67" si="37">Q66/SUM(Q48:Q65)</f>
         <v>1.7937219730941704E-2</v>
       </c>
       <c r="R67">
-        <f t="shared" ref="R67" si="36">R66/SUM(R48:R65)</f>
+        <f t="shared" ref="R67" si="38">R66/SUM(R48:R65)</f>
         <v>1.0563380281690141E-2</v>
       </c>
       <c r="S67">
-        <f t="shared" ref="S67" si="37">S66/SUM(S48:S65)</f>
+        <f t="shared" ref="S67" si="39">S66/SUM(S48:S65)</f>
         <v>3.1446540880503146E-3</v>
       </c>
       <c r="T67">
-        <f t="shared" ref="T67" si="38">T66/SUM(T48:T65)</f>
+        <f t="shared" ref="T67:U67" si="40">T66/SUM(T48:T65)</f>
         <v>7.1260600014252124E-3</v>
       </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U67" s="7">
+        <f t="shared" si="40"/>
+        <v>3.5460992907801418E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>17</v>
       </c>
@@ -8704,79 +9123,83 @@
         <v>1995</v>
       </c>
       <c r="C69">
-        <f t="shared" ref="C69:T69" si="39">C47</f>
+        <f t="shared" ref="C69:T69" si="41">C47</f>
         <v>1996</v>
       </c>
       <c r="D69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>1997</v>
       </c>
       <c r="E69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>1998</v>
       </c>
       <c r="F69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>1999</v>
       </c>
       <c r="G69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2000</v>
       </c>
       <c r="H69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2001</v>
       </c>
       <c r="I69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2002</v>
       </c>
       <c r="J69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2003</v>
       </c>
       <c r="K69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2004</v>
       </c>
       <c r="L69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2005</v>
       </c>
       <c r="M69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2006</v>
       </c>
       <c r="N69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2007</v>
       </c>
       <c r="O69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2008</v>
       </c>
       <c r="P69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2009</v>
       </c>
       <c r="Q69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2010</v>
       </c>
       <c r="R69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2011</v>
       </c>
       <c r="S69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2012</v>
       </c>
       <c r="T69">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2013</v>
       </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U69" s="7">
+        <f t="shared" ref="U69" si="42">U47</f>
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>A48</f>
         <v>00-04</v>
@@ -8857,10 +9280,14 @@
         <f>'newlyacquired-originaldata'!T23+'newlyacquired-originaldata'!T44*0.33</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U70" s="7">
+        <f>'newlyacquired-originaldata'!U23+'newlyacquired-originaldata'!U44*0.33</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f t="shared" ref="A71:A88" si="40">A49</f>
+        <f t="shared" ref="A71:A88" si="43">A49</f>
         <v>05-09</v>
       </c>
       <c r="B71">
@@ -8939,10 +9366,14 @@
         <f>'newlyacquired-originaldata'!T24+'newlyacquired-originaldata'!T45*0.33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U71" s="7">
+        <f>'newlyacquired-originaldata'!U24+'newlyacquired-originaldata'!U45*0.33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>10-14</v>
       </c>
       <c r="B72">
@@ -9021,10 +9452,14 @@
         <f>'newlyacquired-originaldata'!T25+'newlyacquired-originaldata'!T46*0.33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U72" s="7">
+        <f>'newlyacquired-originaldata'!U25+'newlyacquired-originaldata'!U46*0.33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>15-19</v>
       </c>
       <c r="B73">
@@ -9103,10 +9538,14 @@
         <f>'newlyacquired-originaldata'!T26+'newlyacquired-originaldata'!T47*0.33</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U73" s="7">
+        <f>'newlyacquired-originaldata'!U26+'newlyacquired-originaldata'!U47*0.33</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>20-24</v>
       </c>
       <c r="B74">
@@ -9185,10 +9624,14 @@
         <f>'newlyacquired-originaldata'!T27+'newlyacquired-originaldata'!T48*0.33</f>
         <v>31.33</v>
       </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U74" s="7">
+        <f>'newlyacquired-originaldata'!U27+'newlyacquired-originaldata'!U48*0.33</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>25-29</v>
       </c>
       <c r="B75">
@@ -9267,10 +9710,14 @@
         <f>'newlyacquired-originaldata'!T28+'newlyacquired-originaldata'!T49*0.33</f>
         <v>33</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U75" s="7">
+        <f>'newlyacquired-originaldata'!U28+'newlyacquired-originaldata'!U49*0.33</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>30-34</v>
       </c>
       <c r="B76">
@@ -9349,10 +9796,14 @@
         <f>'newlyacquired-originaldata'!T29+'newlyacquired-originaldata'!T50*0.33</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U76" s="7">
+        <f>'newlyacquired-originaldata'!U29+'newlyacquired-originaldata'!U50*0.33</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>35-39</v>
       </c>
       <c r="B77">
@@ -9431,10 +9882,14 @@
         <f>'newlyacquired-originaldata'!T30+'newlyacquired-originaldata'!T51*0.33</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U77" s="7">
+        <f>'newlyacquired-originaldata'!U30+'newlyacquired-originaldata'!U51*0.33</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>40-44</v>
       </c>
       <c r="B78">
@@ -9513,10 +9968,14 @@
         <f>'newlyacquired-originaldata'!T31+'newlyacquired-originaldata'!T52*0.33</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U78" s="7">
+        <f>'newlyacquired-originaldata'!U31+'newlyacquired-originaldata'!U52*0.33</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>45-49</v>
       </c>
       <c r="B79">
@@ -9595,10 +10054,14 @@
         <f>'newlyacquired-originaldata'!T32+'newlyacquired-originaldata'!T53*0.33</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U79" s="7">
+        <f>'newlyacquired-originaldata'!U32+'newlyacquired-originaldata'!U53*0.33</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>50-54</v>
       </c>
       <c r="B80">
@@ -9677,10 +10140,14 @@
         <f>'newlyacquired-originaldata'!T33+'newlyacquired-originaldata'!T54*0.33</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U80" s="7">
+        <f>'newlyacquired-originaldata'!U33+'newlyacquired-originaldata'!U54*0.33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>55-59</v>
       </c>
       <c r="B81">
@@ -9759,10 +10226,14 @@
         <f>'newlyacquired-originaldata'!T34+'newlyacquired-originaldata'!T55*0.33</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U81" s="7">
+        <f>'newlyacquired-originaldata'!U34+'newlyacquired-originaldata'!U55*0.33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>60-64</v>
       </c>
       <c r="B82">
@@ -9841,10 +10312,14 @@
         <f>'newlyacquired-originaldata'!T35+'newlyacquired-originaldata'!T56*0.33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U82" s="7">
+        <f>'newlyacquired-originaldata'!U35+'newlyacquired-originaldata'!U56*0.33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>65-69</v>
       </c>
       <c r="B83">
@@ -9923,10 +10398,14 @@
         <f>'newlyacquired-originaldata'!T36+'newlyacquired-originaldata'!T57*0.33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U83" s="7">
+        <f>'newlyacquired-originaldata'!U36+'newlyacquired-originaldata'!U57*0.33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>70-74</v>
       </c>
       <c r="B84">
@@ -10005,10 +10484,14 @@
         <f>'newlyacquired-originaldata'!T37+'newlyacquired-originaldata'!T58*0.33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U84" s="7">
+        <f>'newlyacquired-originaldata'!U37+'newlyacquired-originaldata'!U58*0.33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>75-79</v>
       </c>
       <c r="B85">
@@ -10087,10 +10570,14 @@
         <f>'newlyacquired-originaldata'!T38+'newlyacquired-originaldata'!T59*0.33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U85" s="7">
+        <f>'newlyacquired-originaldata'!U38+'newlyacquired-originaldata'!U59*0.33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>80-84</v>
       </c>
       <c r="B86">
@@ -10169,10 +10656,14 @@
         <f>'newlyacquired-originaldata'!T39+'newlyacquired-originaldata'!T60*0.33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U86" s="7">
+        <f>'newlyacquired-originaldata'!U39+'newlyacquired-originaldata'!U60*0.33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>85+</v>
       </c>
       <c r="B87">
@@ -10251,10 +10742,14 @@
         <f>'newlyacquired-originaldata'!T40+'newlyacquired-originaldata'!T61*0.33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U87" s="7">
+        <f>'newlyacquired-originaldata'!U40+'newlyacquired-originaldata'!U61*0.33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>Unknown</v>
       </c>
       <c r="B88">
@@ -10333,8 +10828,12 @@
         <f>'newlyacquired-originaldata'!T41+'newlyacquired-originaldata'!T62*0.33</f>
         <v>0.33</v>
       </c>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U88" s="7">
+        <f>'newlyacquired-originaldata'!U41+'newlyacquired-originaldata'!U62*0.33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>24</v>
       </c>
@@ -10343,76 +10842,80 @@
         <v>2.4390243902439025E-2</v>
       </c>
       <c r="C89">
-        <f t="shared" ref="C89" si="41">C88/SUM(C70:C87)</f>
+        <f t="shared" ref="C89" si="44">C88/SUM(C70:C87)</f>
         <v>0</v>
       </c>
       <c r="D89">
-        <f t="shared" ref="D89" si="42">D88/SUM(D70:D87)</f>
+        <f t="shared" ref="D89" si="45">D88/SUM(D70:D87)</f>
         <v>0</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89" si="43">E88/SUM(E70:E87)</f>
+        <f t="shared" ref="E89" si="46">E88/SUM(E70:E87)</f>
         <v>0</v>
       </c>
       <c r="F89">
-        <f t="shared" ref="F89" si="44">F88/SUM(F70:F87)</f>
+        <f t="shared" ref="F89" si="47">F88/SUM(F70:F87)</f>
         <v>0</v>
       </c>
       <c r="G89">
-        <f t="shared" ref="G89" si="45">G88/SUM(G70:G87)</f>
+        <f t="shared" ref="G89" si="48">G88/SUM(G70:G87)</f>
         <v>0</v>
       </c>
       <c r="H89">
-        <f t="shared" ref="H89" si="46">H88/SUM(H70:H87)</f>
+        <f t="shared" ref="H89" si="49">H88/SUM(H70:H87)</f>
         <v>0</v>
       </c>
       <c r="I89">
-        <f t="shared" ref="I89" si="47">I88/SUM(I70:I87)</f>
+        <f t="shared" ref="I89" si="50">I88/SUM(I70:I87)</f>
         <v>0</v>
       </c>
       <c r="J89">
-        <f t="shared" ref="J89" si="48">J88/SUM(J70:J87)</f>
+        <f t="shared" ref="J89" si="51">J88/SUM(J70:J87)</f>
         <v>0</v>
       </c>
       <c r="K89">
-        <f t="shared" ref="K89" si="49">K88/SUM(K70:K87)</f>
+        <f t="shared" ref="K89" si="52">K88/SUM(K70:K87)</f>
         <v>0</v>
       </c>
       <c r="L89">
-        <f t="shared" ref="L89" si="50">L88/SUM(L70:L87)</f>
+        <f t="shared" ref="L89" si="53">L88/SUM(L70:L87)</f>
         <v>2.0121951219512196E-3</v>
       </c>
       <c r="M89">
-        <f t="shared" ref="M89" si="51">M88/SUM(M70:M87)</f>
+        <f t="shared" ref="M89" si="54">M88/SUM(M70:M87)</f>
         <v>0</v>
       </c>
       <c r="N89">
-        <f t="shared" ref="N89" si="52">N88/SUM(N70:N87)</f>
+        <f t="shared" ref="N89" si="55">N88/SUM(N70:N87)</f>
         <v>0</v>
       </c>
       <c r="O89">
-        <f t="shared" ref="O89" si="53">O88/SUM(O70:O87)</f>
+        <f t="shared" ref="O89" si="56">O88/SUM(O70:O87)</f>
         <v>0</v>
       </c>
       <c r="P89">
-        <f t="shared" ref="P89" si="54">P88/SUM(P70:P87)</f>
+        <f t="shared" ref="P89" si="57">P88/SUM(P70:P87)</f>
         <v>0</v>
       </c>
       <c r="Q89">
-        <f t="shared" ref="Q89" si="55">Q88/SUM(Q70:Q87)</f>
+        <f t="shared" ref="Q89" si="58">Q88/SUM(Q70:Q87)</f>
         <v>0</v>
       </c>
       <c r="R89">
-        <f t="shared" ref="R89" si="56">R88/SUM(R70:R87)</f>
+        <f t="shared" ref="R89" si="59">R88/SUM(R70:R87)</f>
         <v>0</v>
       </c>
       <c r="S89">
-        <f t="shared" ref="S89" si="57">S88/SUM(S70:S87)</f>
+        <f t="shared" ref="S89" si="60">S88/SUM(S70:S87)</f>
         <v>5.9281437125748501E-3</v>
       </c>
       <c r="T89">
-        <f t="shared" ref="T89" si="58">T88/SUM(T70:T87)</f>
+        <f t="shared" ref="T89:U89" si="61">T88/SUM(T70:T87)</f>
         <v>2.5320340673674522E-3</v>
+      </c>
+      <c r="U89" s="7">
+        <f t="shared" si="61"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -10422,15 +10925,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T62"/>
+  <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:T41"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="U44" sqref="U44:U62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -10491,8 +10994,11 @@
       <c r="T1">
         <v>2013</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -10553,8 +11059,11 @@
       <c r="T2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -10615,8 +11124,11 @@
       <c r="T3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -10677,8 +11189,11 @@
       <c r="T4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -10739,8 +11254,11 @@
       <c r="T5">
         <v>158</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -10801,8 +11319,11 @@
       <c r="T6">
         <v>611</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -10863,8 +11384,11 @@
       <c r="T7">
         <v>777</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -10925,8 +11449,11 @@
       <c r="T8">
         <v>935</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -10987,8 +11514,11 @@
       <c r="T9">
         <v>868</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -11049,8 +11579,11 @@
       <c r="T10">
         <v>851</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -11111,8 +11644,11 @@
       <c r="T11">
         <v>811</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -11173,8 +11709,11 @@
       <c r="T12">
         <v>711</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -11235,8 +11774,11 @@
       <c r="T13">
         <v>571</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -11297,8 +11839,11 @@
       <c r="T14">
         <v>263</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -11359,8 +11904,11 @@
       <c r="T15">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -11421,8 +11969,11 @@
       <c r="T16">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -11483,8 +12034,11 @@
       <c r="T17">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -11545,8 +12099,11 @@
       <c r="T18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -11607,8 +12164,11 @@
       <c r="T19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -11669,8 +12229,11 @@
       <c r="T20">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -11679,7 +12242,7 @@
         <v>1995</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:T22" si="0">C1</f>
+        <f t="shared" ref="C22:U22" si="0">C1</f>
         <v>1996</v>
       </c>
       <c r="D22">
@@ -11750,8 +12313,12 @@
         <f t="shared" si="0"/>
         <v>2013</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U22" s="5">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>A2</f>
         <v>00-04</v>
@@ -11813,8 +12380,11 @@
       <c r="T23">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" ref="A24:A41" si="1">A3</f>
         <v>05-09</v>
@@ -11876,8 +12446,11 @@
       <c r="T24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="1"/>
         <v>10-14</v>
@@ -11939,8 +12512,11 @@
       <c r="T25">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="1"/>
         <v>15-19</v>
@@ -12002,8 +12578,11 @@
       <c r="T26">
         <v>120</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U26">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="1"/>
         <v>20-24</v>
@@ -12065,8 +12644,11 @@
       <c r="T27">
         <v>329</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U27">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="1"/>
         <v>25-29</v>
@@ -12128,8 +12710,11 @@
       <c r="T28">
         <v>379</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="1"/>
         <v>30-34</v>
@@ -12191,8 +12776,11 @@
       <c r="T29">
         <v>585</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U29">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="1"/>
         <v>35-39</v>
@@ -12254,8 +12842,11 @@
       <c r="T30">
         <v>449</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U30">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="1"/>
         <v>40-44</v>
@@ -12317,8 +12908,11 @@
       <c r="T31">
         <v>379</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U31">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="1"/>
         <v>45-49</v>
@@ -12380,8 +12974,11 @@
       <c r="T32">
         <v>353</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U32">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="1"/>
         <v>50-54</v>
@@ -12443,8 +13040,11 @@
       <c r="T33">
         <v>367</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U33">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="1"/>
         <v>55-59</v>
@@ -12506,8 +13106,11 @@
       <c r="T34">
         <v>283</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U34">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="1"/>
         <v>60-64</v>
@@ -12569,8 +13172,11 @@
       <c r="T35">
         <v>117</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="1"/>
         <v>65-69</v>
@@ -12632,8 +13238,11 @@
       <c r="T36">
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U36">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="1"/>
         <v>70-74</v>
@@ -12695,8 +13304,11 @@
       <c r="T37">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U37">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="1"/>
         <v>75-79</v>
@@ -12758,8 +13370,11 @@
       <c r="T38">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="1"/>
         <v>80-84</v>
@@ -12821,8 +13436,11 @@
       <c r="T39">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U39">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="1"/>
         <v>85+</v>
@@ -12884,8 +13502,11 @@
       <c r="T40">
         <v>22</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U40">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="1"/>
         <v>Unknown</v>
@@ -12947,8 +13568,11 @@
       <c r="T41">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -12957,7 +13581,7 @@
         <v>1995</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:T43" si="2">C22</f>
+        <f t="shared" ref="C43:U43" si="2">C22</f>
         <v>1996</v>
       </c>
       <c r="D43">
@@ -13028,8 +13652,12 @@
         <f t="shared" si="2"/>
         <v>2013</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U43" s="6">
+        <f t="shared" si="2"/>
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>A23</f>
         <v>00-04</v>
@@ -13091,8 +13719,11 @@
       <c r="T44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" ref="A45:A62" si="3">A24</f>
         <v>05-09</v>
@@ -13154,8 +13785,11 @@
       <c r="T45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="3"/>
         <v>10-14</v>
@@ -13217,8 +13851,11 @@
       <c r="T46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="3"/>
         <v>15-19</v>
@@ -13280,8 +13917,11 @@
       <c r="T47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="3"/>
         <v>20-24</v>
@@ -13343,8 +13983,11 @@
       <c r="T48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="3"/>
         <v>25-29</v>
@@ -13406,8 +14049,11 @@
       <c r="T49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="3"/>
         <v>30-34</v>
@@ -13469,8 +14115,11 @@
       <c r="T50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="3"/>
         <v>35-39</v>
@@ -13532,8 +14181,11 @@
       <c r="T51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="3"/>
         <v>40-44</v>
@@ -13595,8 +14247,11 @@
       <c r="T52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="3"/>
         <v>45-49</v>
@@ -13658,8 +14313,11 @@
       <c r="T53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="3"/>
         <v>50-54</v>
@@ -13721,8 +14379,11 @@
       <c r="T54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="3"/>
         <v>55-59</v>
@@ -13784,8 +14445,11 @@
       <c r="T55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="3"/>
         <v>60-64</v>
@@ -13847,8 +14511,11 @@
       <c r="T56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f t="shared" si="3"/>
         <v>65-69</v>
@@ -13910,8 +14577,11 @@
       <c r="T57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="3"/>
         <v>70-74</v>
@@ -13973,8 +14643,11 @@
       <c r="T58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="3"/>
         <v>75-79</v>
@@ -14036,8 +14709,11 @@
       <c r="T59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="3"/>
         <v>80-84</v>
@@ -14099,8 +14775,11 @@
       <c r="T60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="3"/>
         <v>85+</v>
@@ -14162,8 +14841,11 @@
       <c r="T61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="3"/>
         <v>Unknown</v>
@@ -14224,6 +14906,9 @@
       </c>
       <c r="T62">
         <v>2</v>
+      </c>
+      <c r="U62">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -14233,15 +14918,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T62"/>
+  <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U44" sqref="U44:U62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -14302,8 +14987,11 @@
       <c r="T1">
         <v>2013</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -14364,8 +15052,11 @@
       <c r="T2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -14426,8 +15117,11 @@
       <c r="T3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -14488,8 +15182,11 @@
       <c r="T4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -14550,8 +15247,11 @@
       <c r="T5">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -14612,8 +15312,11 @@
       <c r="T6">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -14674,8 +15377,11 @@
       <c r="T7">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -14736,8 +15442,11 @@
       <c r="T8">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -14798,8 +15507,11 @@
       <c r="T9">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -14860,8 +15572,11 @@
       <c r="T10">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -14922,8 +15637,11 @@
       <c r="T11">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -14984,8 +15702,11 @@
       <c r="T12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -15046,8 +15767,11 @@
       <c r="T13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -15108,8 +15832,11 @@
       <c r="T14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -15170,8 +15897,11 @@
       <c r="T15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -15232,8 +15962,11 @@
       <c r="T16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -15294,8 +16027,11 @@
       <c r="T17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -15356,8 +16092,11 @@
       <c r="T18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -15418,8 +16157,11 @@
       <c r="T19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -15480,8 +16222,11 @@
       <c r="T20">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -15490,7 +16235,7 @@
         <v>1995</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:T22" si="0">C1</f>
+        <f t="shared" ref="C22:U22" si="0">C1</f>
         <v>1996</v>
       </c>
       <c r="D22">
@@ -15561,8 +16306,12 @@
         <f t="shared" si="0"/>
         <v>2013</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U22" s="3">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>A2</f>
         <v>00-04</v>
@@ -15624,8 +16373,11 @@
       <c r="T23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" ref="A24:A41" si="1">A3</f>
         <v>05-09</v>
@@ -15687,8 +16439,11 @@
       <c r="T24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="1"/>
         <v>10-14</v>
@@ -15750,8 +16505,11 @@
       <c r="T25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="1"/>
         <v>15-19</v>
@@ -15813,8 +16571,11 @@
       <c r="T26">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="1"/>
         <v>20-24</v>
@@ -15876,8 +16637,11 @@
       <c r="T27">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U27">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="1"/>
         <v>25-29</v>
@@ -15939,8 +16703,11 @@
       <c r="T28">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="1"/>
         <v>30-34</v>
@@ -16002,8 +16769,11 @@
       <c r="T29">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="1"/>
         <v>35-39</v>
@@ -16065,8 +16835,11 @@
       <c r="T30">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="1"/>
         <v>40-44</v>
@@ -16128,8 +16901,11 @@
       <c r="T31">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="1"/>
         <v>45-49</v>
@@ -16191,8 +16967,11 @@
       <c r="T32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="1"/>
         <v>50-54</v>
@@ -16254,8 +17033,11 @@
       <c r="T33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="1"/>
         <v>55-59</v>
@@ -16317,8 +17099,11 @@
       <c r="T34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="1"/>
         <v>60-64</v>
@@ -16380,8 +17165,11 @@
       <c r="T35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="1"/>
         <v>65-69</v>
@@ -16443,8 +17231,11 @@
       <c r="T36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="1"/>
         <v>70-74</v>
@@ -16506,8 +17297,11 @@
       <c r="T37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="1"/>
         <v>75-79</v>
@@ -16569,8 +17363,11 @@
       <c r="T38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="1"/>
         <v>80-84</v>
@@ -16632,8 +17429,11 @@
       <c r="T39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="1"/>
         <v>85+</v>
@@ -16695,8 +17495,11 @@
       <c r="T40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="1"/>
         <v>Unknown</v>
@@ -16758,8 +17561,11 @@
       <c r="T41">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -16768,7 +17574,7 @@
         <v>1995</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:T43" si="2">C22</f>
+        <f t="shared" ref="C43:U43" si="2">C22</f>
         <v>1996</v>
       </c>
       <c r="D43">
@@ -16839,8 +17645,12 @@
         <f t="shared" si="2"/>
         <v>2013</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U43" s="4">
+        <f t="shared" si="2"/>
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>A23</f>
         <v>00-04</v>
@@ -16902,8 +17712,11 @@
       <c r="T44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" ref="A45:A62" si="3">A24</f>
         <v>05-09</v>
@@ -16965,8 +17778,11 @@
       <c r="T45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="3"/>
         <v>10-14</v>
@@ -17028,8 +17844,11 @@
       <c r="T46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="3"/>
         <v>15-19</v>
@@ -17091,8 +17910,11 @@
       <c r="T47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="3"/>
         <v>20-24</v>
@@ -17154,8 +17976,11 @@
       <c r="T48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" si="3"/>
         <v>25-29</v>
@@ -17217,8 +18042,11 @@
       <c r="T49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="3"/>
         <v>30-34</v>
@@ -17280,8 +18108,11 @@
       <c r="T50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="3"/>
         <v>35-39</v>
@@ -17343,8 +18174,11 @@
       <c r="T51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="3"/>
         <v>40-44</v>
@@ -17406,8 +18240,11 @@
       <c r="T52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="3"/>
         <v>45-49</v>
@@ -17469,8 +18306,11 @@
       <c r="T53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="3"/>
         <v>50-54</v>
@@ -17532,8 +18372,11 @@
       <c r="T54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="3"/>
         <v>55-59</v>
@@ -17595,8 +18438,11 @@
       <c r="T55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="3"/>
         <v>60-64</v>
@@ -17658,8 +18504,11 @@
       <c r="T56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f t="shared" si="3"/>
         <v>65-69</v>
@@ -17721,8 +18570,11 @@
       <c r="T57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="3"/>
         <v>70-74</v>
@@ -17784,8 +18636,11 @@
       <c r="T58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="3"/>
         <v>75-79</v>
@@ -17847,8 +18702,11 @@
       <c r="T59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="3"/>
         <v>80-84</v>
@@ -17910,8 +18768,11 @@
       <c r="T60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="3"/>
         <v>85+</v>
@@ -17973,8 +18834,11 @@
       <c r="T61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="3"/>
         <v>Unknown</v>
@@ -18035,6 +18899,9 @@
       </c>
       <c r="T62">
         <v>1</v>
+      </c>
+      <c r="U62">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>